<commit_message>
🗃️ change excels data
</commit_message>
<xml_diff>
--- a/data/dataset_RAG_improvment.xlsx
+++ b/data/dataset_RAG_improvment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maicolrodrigues/Documents/Test/Insurapolis/chatbot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79802C31-AFF9-1D40-83F1-D14B840C8A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B966B9DA-59D8-7448-A8AE-6379E897424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70900" yWindow="-10300" windowWidth="46220" windowHeight="27840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44020" yWindow="-10300" windowWidth="55380" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t>index</t>
   </si>
@@ -156,18 +156,6 @@
     <t>Art. 106</t>
   </si>
   <si>
-    <t>Art. 107 
-Incendie
-107.1 Étendue de l’assurance
-Sont assurés 
-• les dommages causés par un incendie, l’action soudaine et accidentelle de la fumée, la foudre, une explosion et une implosion, la chute ou l’atterrissage forcé d’aéronefs et de vaisseaux spatiaux ou de parties qui s’en détachent;
-• les dommages causés par des travaux d’extinction et de déblaiement;
-• disparition consécutive à ces événements:
-• les dommages de roussissement et les dommages aux choses assurées exposées involontairement à la chaleur.
-107.2 Restrictions de l’étendue de l’assurance
-Sont exclus de l’assurance les dommages causés à des machines, appareils et conduites sous tension par l’effet propre de l’électricité.</t>
-  </si>
-  <si>
     <t>Art. 107</t>
   </si>
   <si>
@@ -187,23 +175,6 @@
   </si>
   <si>
     <t>Art. 108</t>
-  </si>
-  <si>
-    <t>Art. 109 
-Tremblements de terre et éruptions volcaniques
-109.1 Étendue de l’assurance
-Sont assurés les endommagements, les destructions ou la perte de choses assurées qui sont la conséquence directe ou indirecte de tremblements de terreou d’érup-
-tions volcaniques.
-En dérogation aux exclusions générales énoncées à l’art. 106, les actes de pillage se produisant à la suite d’un tremblement de terre ou d’une éruption volcanique sont coassurés. On entend par tremblement de terre des secousses violentes du sol provoquées par des phénomènes tectoniques naturels dans l’écorce terrestre et le manteau supérieur. S’il n’est pas possible de déterminer exactement s’il s’agit d’un tremblement de terre, l’avis du Service sismologique suisse (SSS) est déterminant.
-On entend par éruption volcanique l’évacuation de la pression lors de la formation d’une crevasse, associée à des coulées de laves, à l’éruption de cendres ou d’autres matières et gaz se libérant.
-109.2 Validité temporelle
-Tous les tremblements de terre ou éruptions volcaniques qui surviennent dans les 168 heures après la secousse resp. l’éruption ayant provoqué les premiers dommages constituent un seul cas de sinistre.
-Sont assurés tous les sinistres dont l’origine se situe pendant la durée de l’assurance.
-109.3 Prétentions envers des tiers et d’autres fournisseurs de prestations
-Si Zurich fournit des prestations pour des droits aux prestations que les ayants droit peuvent faire valoir auprès de tiers, lesdites prétentions de ce contrat sont cédées à Zurich au moment de la fourniture des prestations.
-En cas d’assurance obligatoire contre les tremblements de terre ou les éruptions volcaniques auprès d’une institution d’assurance cantonale, il est possible, en complément des prestations versées par cette dernière, de faire valoir par le biais du présent contrat un éventuel dommage résiduel.
-109.4 Résiliation
-En dérogation à l’art. 2.1, chaque partie au contrat peut résilier la prestation «Tremblements de terre et éruptions volcaniques», en respectant un délai de trois mois, à l’échéance de chaque année d’assurance, par écrit ou sous une autre forme permettant d’en établir la preuve par un texte.</t>
   </si>
   <si>
     <t>Art. 109</t>
@@ -256,6 +227,9 @@
     <t>Art. 112</t>
   </si>
   <si>
+    <t>Art. 113</t>
+  </si>
+  <si>
     <t>Art. 113 
 Prestations
 113.1 Valeur de remplacement et calcul du dommage
@@ -265,13 +239,10 @@
 113.2.2 Somme d’assurance pour les valeurs pécuniaires
 a) Prestation d’assurance «CLASSIC»
 Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par l’incendie, les événements naturels, le vol avec effraction, le détroussement, les tremblements de terre, les éruptions volcaniques et le dégât d’eau, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
-Dans le cadre du risque spécial «inventaire du ménage dans trésor bancaire», les valeurs pécuniaires sont assurées à concurrence de la somme d’assurance convenue 
-dans la police.
-En cas de vol simple, aucune prestation n’est fournie.
+Dans le cadre du risque spécial «inventaire du ménage dans trésor bancaire», les valeurs pécuniaires sont assurées à concurrence de la somme d’assurance convenue dans la police. En cas de vol simple, aucune prestation n’est fournie.
 113.2.3 Limitation des prestations pour les dommages de roussissement
 a) Prestation d’assurance «CLASSIC»
-Les prestations pour les dommages de roussissement et les dommages causés à des choses assurées, qui ont été exposées involontairement à la chaleur, s’élèvent au 
-maximum à CHF 5’000.
+Les prestations pour les dommages de roussissement et les dommages causés à des choses assurées, qui ont été exposées involontairement à la chaleur, s’élèvent au maximum à CHF 5’000.
 a) Prestation d’assurance «CLASSIC»
 Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causés par l’incendie, les événements naturels, les tremblements de terre et éruptions volcaniques, le vol et le dégât d’eau, si ces événements sont mentionnés dans la police.
 113.2.5 Somme d’assurance pour les objets de remplacement en cas de retard des bagages
@@ -281,33 +252,63 @@
 Les choses récupérées ultérieurement doivent être remises à Zurich ou l’indemnisation fournie doit être remboursée.</t>
   </si>
   <si>
-    <t>Art. 113</t>
-  </si>
-  <si>
-    <t>Art. 113 
-Prestations
+    <r>
+      <t xml:space="preserve">Art. 111 
+Dégâts d’eau
+111.1 Étendue de l’assurance
+Sont assurés les dommages causés par:
+• des liquides et des gaz s’écoulant des conduites et installations desservant les bâtiments aux lieux assurés, des liquides et des gaz s’écoulant des installations et appareils qui y sont raccordés et d’autres appareils et installations aquifères tels qu’aquariums, fontaines, humidificateurs d’air et matelas d’eau,
+• l’eau de pluie, l’eau de la fonte de neige et de glace qui s’infiltre dans le bâtiment,
+• les dommages à l’intérieur du bâtiment causés par le refoulement des canalisations d’écoulement ou le ruissellement des eaux souterraines.
+Sont également assurés:
+• la disparition de choses assurées consécutive à ces événements;
+• les frais de réparation de conduites d’eau endommagées par le gel ou le dégèlement de conduites d’eau, compteurs d’eau inclus, et des appareils qui y sont raccordés que le locataire a installés à l’intérieur du bâtiment.
+111.2 Restrictions de l’étendue de l’assurance
+Sont exclus de l’assurance les dommages
+• qui sont assurés dans le cadre d’événements incendie et dommages naturels,
+• causés par l’infiltration d’eau de pluie, d’eau de fonte de neige ou de glace par des lucarnes, des fenêtres et portes ouvertes ou des ouvertures dans le toit ou dans les murs de nouvelles constructions ou dans le cadre de travaux de transformation ou autres du bâtiment,
+• causés lors du remplissage et lors de la réparation ou la révision d’installations de chauffage et de citernes ainsi que d’échangeurs thermiques et/ou de pompes à chaleur en circuit fermé.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Art. 113 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Prestations
 113.1 Valeur de remplacement et calcul du dommage
 Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
 113.2 Sommes d’assurance et limitations des prestations
 La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
 113.2.2 Somme d’assurance pour les valeurs pécuniaires
-b) Prestation d’assurance «ALL RISK»
-Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par les événements All Risk, tremblements de terre et éruptions 
-volcaniques, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
-113.2.3 Limitation des prestations pour les dommages de roussissement
-b) Prestation d’assurance «ALL RISK»
-Il n’existe pas de limitations particulières des prestations pour les dommages de roussissement et les dommages causés à des choses assurées qui ont été exposées involontairement à la chaleur.
-113.2.4 Somme d’assurance pour les effets d’hôtes et les objets confiés
-b) Prestation d’assurance «ALL RISK»
-Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les événements All Risk, les tremblements de terre et les éruptions volcaniques, si ces événements sont mentionnés dans la police.
-113.2.5 Somme d’assurance pour les objets de remplacement en cas de retard des bagages
-b) Prestation d’assurance «ALL RISK»
-Si les bagages confiés à un transporteur sont livrés en retard, les frais d’achat d’objets de remplacement absolument nécessaires sont couverts au premier risque jusqu’à CHF 2’000.
-113.3 Choses récupérées
-Les choses récupérées ultérieurement doivent être remises à Zurich ou l’indemnisation fournie doit être remboursée.</t>
-  </si>
-  <si>
-    <t>Art. 110 
+a) Prestation d’assurance «CLASSIC»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés le dégât d’eau, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+a) Prestation d’assurance «CLASSIC»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causés par le dégât d’eau, si ces événements sont mentionnés dans la police.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 110 
 Vol
 110.1 Étendue de l’assurance
 Sont assurés les dommages causés par les événements suivants, dans la mesure où ces événements sont prouvés par des traces, des témoins ou, selon les circonstances, d’une autre manière probante.
@@ -332,10 +333,218 @@
 En cas de vol simple «à la maison» selon l’art. 102.2.1 et en cas de vol avec effraction en général (pas en cas de détroussement), la prestation versée pour les bijoux est limitée à 20% de la somme d’assurance, au maximum CHF 30’000. Cette restriction ne s’applique pas si les bijoux sont enfermés dans un coffre-fort d’un poids total d’au moins 100 kg ou dans un coffre emmuré et que les clés ou les codes de serrures à combinaison sont conservés soigneusement ou que les personnes responsables les portent sur elles.
 c) Prestation d’assurance «CLASSIC» 
 • Dans les maisons de vacances, les appartements de vacances et les résidences (appartements) secondaires non habités, les bijoux sont assurés en cas de vol uniquement s’ils sont enfermés dans un coffre-fort d’un poids total d’au moins 100 kg ou dans un coffre emmuré et que les clés ou codes de serrures à combinaison  sont conservés soigneusement à un autre endroit ou que les personnes responsables les portent sur elles. Dans ces conditions, la prestation pour les bijoux dans ces lieux est limitée à CHF 100’000. 
-• Les montres-bracelets et montres de poche ayant une valeur unitaire supérieure à CHF 5’000 sont considérées comme des bijoux.</t>
-  </si>
-  <si>
-    <t>Art. 110 
+• Les montres-bracelets et montres de poche ayant une valeur unitaire supérieure à CHF 5’000 sont considérées comme des bijoux.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Art. 113 
+Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+a) Prestation d’assurance «CLASSIC»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre le vol avec effraction, le détroussement,  si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Dans le cadre du risque spécial «inventaire du ménage dans trésor bancaire», les valeurs pécuniaires sont assurées à concurrence de la somme d’assurance convenue dans la police. En cas de vol simple, aucune prestation n’est fournie.
+a) Prestation d’assurance «CLASSIC»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causés par  le vol si cet evenement est mentionné dans la police.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 109 
+Tremblements de terre et éruptions volcaniques
+109.1 Étendue de l’assurance
+Sont assurés les endommagements, les destructions ou la perte de choses assurées qui sont la conséquence directe ou indirecte de tremblements de terreou d’érup-
+tions volcaniques.
+En dérogation aux exclusions générales énoncées à l’art. 106, les actes de pillage se produisant à la suite d’un tremblement de terre ou d’une éruption volcanique sont coassurés. On entend par tremblement de terre des secousses violentes du sol provoquées par des phénomènes tectoniques naturels dans l’écorce terrestre et le manteau supérieur. S’il n’est pas possible de déterminer exactement s’il s’agit d’un tremblement de terre, l’avis du Service sismologique suisse (SSS) est déterminant.
+On entend par éruption volcanique l’évacuation de la pression lors de la formation d’une crevasse, associée à des coulées de laves, à l’éruption de cendres ou d’autres matières et gaz se libérant.
+109.2 Validité temporelle
+Tous les tremblements de terre ou éruptions volcaniques qui surviennent dans les 168 heures après la secousse resp. l’éruption ayant provoqué les premiers dommages constituent un seul cas de sinistre.
+Sont assurés tous les sinistres dont l’origine se situe pendant la durée de l’assurance.
+109.3 Prétentions envers des tiers et d’autres fournisseurs de prestations
+Si Zurich fournit des prestations pour des droits aux prestations que les ayants droit peuvent faire valoir auprès de tiers, lesdites prétentions de ce contrat sont cédées à Zurich au moment de la fourniture des prestations.
+En cas d’assurance obligatoire contre les tremblements de terre ou les éruptions volcaniques auprès d’une institution d’assurance cantonale, il est possible, en complément des prestations versées par cette dernière, de faire valoir par le biais du présent contrat un éventuel dommage résiduel.
+109.4 Résiliation
+En dérogation à l’art. 2.1, chaque partie au contrat peut résilier la prestation «Tremblements de terre et éruptions volcaniques», en respectant un délai de trois mois, à l’échéance de chaque année d’assurance, par écrit ou sous une autre forme permettant d’en établir la preuve par un texte.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Art. 113 
+Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+a) Prestation d’assurance «CLASSIC»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les événements naturels, les tremblements de terre, les éruptions volcaniques, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+a) Prestation d’assurance «CLASSIC»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causés par les tremblements de terre et éruptions volcaniques, si ces événements sont mentionnés dans la police.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 108 
+Événements naturels
+108.1 Étendue de l’assurance
+Sont assurés les dommages causés par des hautes eaux, des inondations, des tempêtes (vent d’au moins 75 km/h qui renverse les arbres et découvre les maisons dans le voisinage des choses assurées), la grêle, des avalanches, la pression de la neige, un éboulement de rochers, des chutes de pierres et des glissements de terrain. La disparition de choses assurées consécutive à ces événements est également assurée.
+108.2 Restrictions de l’étendue de l’assurance 
+a) Ne sont pas des dommages dus aux événements naturels:
+– les dommages causés par un affaissement de terrain, le mauvais état d’un terrain à bâtir, une construction défectueuse, l’entretien défectueux des bâtiments, l’omission de mesures de défense, les mouvements de terrain dus à des travaux, le  glissement de la neige des toits, les eaux souterraines ainsi que la crue et le débordement de cours ou de nappes d’eau dont on sait par expérience qu’ils se répètent à intervalles plus ou moins longs;
+– les dommages dus à l’eau de lacs artificiels ou d’autres installations hydrauliques, au refoulement des eaux de canalisation et aux modifications de la  structure de l’atome, sans égard à leur cause;
+– les dommages d’exploitation avec lesquels il faut compter, au vu des expériences faites, tels ceux qui surviennent lors de travaux de génie civil et en matière de bâtiments, lors de la construction de galeries et lors de l’extraction de pierres, de gravier, de sable ou d’argile;
+– les dommages causés par des secousses ayant leur cause dans l’effondrement de vides créés artificiellement;
+– les dommages causés par les secousses déclenchées par des processus tectoniques dans la croûte terrestre (tremblements de terre) et les éruptions volcaniques.
+b) Sont exclus de l’assurance des dommages dus à des événements  naturels:
+– les dommages dus aux tempêtes et à l’eau que subissent les  bateaux lorsqu’ils se trouvent sur l’eau.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Art. 113 
+Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+a) Prestation d’assurance «CLASSIC»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par les événements naturels, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+a) Prestation d’assurance «CLASSIC»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causé les événements naturels, si ces événements sont mentionnés dans la police.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 107 
+Incendie
+107.1 Étendue de l’assurance
+Sont assurés 
+• les dommages causés par un incendie, l’action soudaine et accidentelle de la fumée, la foudre, une explosion et une implosion, la chute ou l’atterrissage forcé d’aéronefs et de vaisseaux spatiaux ou de parties qui s’en détachent;
+• les dommages causés par des travaux d’extinction et de déblaiement;
+• disparition consécutive à ces événements:
+• les dommages de roussissement et les dommages aux choses assurées exposées involontairement à la chaleur.
+107.2 Restrictions de l’étendue de l’assurance
+Sont exclus de l’assurance les dommages causés à des machines, appareils et conduites sous tension par l’effet propre de l’électricité.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Art. 113 
+Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+a) Prestation d’assurance «CLASSIC»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par l’incendie, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+113.2.3 Limitation des prestations pour les dommages de roussissement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="6"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>a) Prestation d’assurance «CLASSIC»
+Les prestations pour les dommages de roussissement et les dommages causés à des choses assurées, qui ont été exposées involontairement à la chaleur, s’élèvent au maximum à CHF 5’000.
+a) Prestation d’assurance «CLASSIC»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les dommages causés par l’incendie, si cet événement est mentionné dans la police.</t>
+    </r>
+  </si>
+  <si>
+    <t>Art. 113 
+Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+b) Prestation d’assurance «ALL RISK»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par les événements All Risk, tremblements de terre et éruptions volcaniques, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+113.2.3 Limitation des prestations pour les dommages de roussissement
+b) Prestation d’assurance «ALL RISK»
+Il n’existe pas de limitations particulières des prestations pour les dommages de roussissement et les dommages causés à des choses assurées qui ont été exposées involontairement à la chaleur.
+113.2.4 Somme d’assurance pour les effets d’hôtes et les objets confiés
+b) Prestation d’assurance «ALL RISK»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les événements All Risk, les tremblements de terre et les éruptions volcaniques, si ces événements sont mentionnés dans la police.
+113.2.5 Somme d’assurance pour les objets de remplacement en cas de retard des bagages
+b) Prestation d’assurance «ALL RISK»
+Si les bagages confiés à un transporteur sont livrés en retard, les frais d’achat d’objets de remplacement absolument nécessaires sont couverts au premier risque jusqu’à CHF 2’000.
+113.3 Choses récupérées
+Les choses récupérées ultérieurement doivent être remises à Zurich ou l’indemnisation fournie doit être remboursée.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 109 
+Tremblements de terre et éruptions volcaniques
+109.1 Étendue de l’assurance
+Sont assurés les endommagements, les destructions ou la perte de choses assurées qui sont la conséquence directe ou indirecte de tremblements de terreou d’érup-
+tions volcaniques.
+En dérogation aux exclusions générales énoncées à l’art. 106, les actes de pillage se produisant à la suite d’un tremblement de terre ou d’une éruption volcanique sont coassurés. On entend par tremblement de terre des secousses violentes du sol provoquées par des phénomènes tectoniques naturels dans l’écorce terrestre et le manteau supérieur. S’il n’est pas possible de déterminer exactement s’il s’agit d’un tremblement de terre, l’avis du Service sismologique suisse (SSS) est déterminant.
+On entend par éruption volcanique l’évacuation de la pression lors de la formation d’une crevasse, associée à des coulées de laves, à l’éruption de cendres ou d’autres matières et gaz se libérant.
+109.2 Validité temporelle
+Tous les tremblements de terre ou éruptions volcaniques qui surviennent dans les 168 heures après la secousse resp. l’éruption ayant provoqué les premiers dommages constituent un seul cas de sinistre.
+Sont assurés tous les sinistres dont l’origine se situe pendant la durée de l’assurance.
+109.3 Prétentions envers des tiers et d’autres fournisseurs de prestations
+Si Zurich fournit des prestations pour des droits aux prestations que les ayants droit peuvent faire valoir auprès de tiers, lesdites prétentions de ce contrat sont cédées à Zurich au moment de la fourniture des prestations.
+En cas d’assurance obligatoire contre les tremblements de terre ou les éruptions volcaniques auprès d’une institution d’assurance cantonale, il est possible, en complément des prestations versées par cette dernière, de faire valoir par le biais du présent contrat un éventuel dommage résiduel.
+109.4 Résiliation
+En dérogation à l’art. 2.1, chaque partie au contrat peut résilier la prestation «Tremblements de terre et éruptions volcaniques», en respectant un délai de trois mois, à l’échéance de chaque année d’assurance, par écrit ou sous une autre forme permettant d’en établir la preuve par un texte.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Prestations
+113.1 Valeur de remplacement et calcul du dommage
+Pour l’inventaire du ménage, les effets d’hôtes et les objets confiés, le dommage est calculé à partir du montant du remplacement à la valeur à neuf au moment du cas de sinistre (= valeur de remplacement), déduction faite de la valeur des restes. Une valeur d’amateur personnelle n’est pas prise en considération. En cas de dommage partiel, le dommage est calculé à partir des frais de réparation à  concurrence de la valeur de remplacement.
+113.2 Sommes d’assurance et limitations des prestations
+La somme d’assurance constitue la limite d’indemnisation, dans la mesure où certaines limitations de prestations particulières ne sont pas applicables. Pour les dommages relevant du champ d’application de l’assurance des dommages naturels légale, les dispositions légales mentionnées à l’art. 17 s’appliquent.
+113.2.2 Somme d’assurance pour les valeurs pécuniaires
+b) Prestation d’assurance «ALL RISK»
+Les valeurs pécuniaires sont assurées au premier risque jusqu’à CHF 5’000 contre les dommages causés par les événements All Risk, tremblements de terre et éruptions volcaniques, si ces événements sont mentionnés dans la police et si une somme d’assurance plus élevée n’a pas été convenue.
+b) Prestation d’assurance «ALL RISK»
+Les effets d’hôtes (sans valeurs pécuniaires ni bijoux) et les objets confiés sont assurés au premier risque jusqu’à CHF 5’000 contre les événements All Risk, les tremblements de terre et les éruptions volcaniques, si ces événements sont mentionnés dans la police.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 110 
 Vol
 110.1 Étendue de l’assurance
 Sont assurés les dommages causés par les événements suivants, dans la mesure où ces événements sont prouvés par des traces, des témoins ou, selon les circonstances, d’une autre manière probante.
@@ -364,14 +573,51 @@
 c) Prestation d’assurance «ALL RISK»
 • Dans les maisons de vacances, les appartements de vacances et les résidences (appartements) secondaires non habités, les bijoux sont assurés en cas de vol uniquement s’ils sont enfermés dans un coffre-fort d’un poids total d’au moins 100 kg ou dans un coffre emmuré et que les clés ou codes de serrures à combinaison  sont conservés soigneusement à un autre endroit ou que les personnes responsables les portent sur elles. 
 Dans ces conditions, la prestation pour les bijoux dans ces lieux est limitée à CHF 100’000. 
-• Les montres-bracelets et montres de poche ayant une valeur unitaire supérieure à CHF 5’000 sont considérées comme des bijoux.</t>
+• Les montres-bracelets et montres de poche ayant une valeur unitaire supérieure à CHF 5’000 sont considérées comme des bijoux.
+Si les bagages confiés à un transporteur sont livrés en retard, les frais d’achat d’objets de remplacement absolument nécessaires sont couverts au premier risque jusqu’à CHF 2’000.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>113.3 Choses récupérées
+Les choses récupérées ultérieurement doivent être remises à Zurich ou l’indemnisation fournie doit être remboursée.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Art. 107 
+Incendie
+107.1 Étendue de l’assurance
+Sont assurés 
+• les dommages causés par un incendie, l’action soudaine et accidentelle de la fumée, la foudre, une explosion et une implosion, la chute ou l’atterrissage forcé d’aéronefs et de vaisseaux spatiaux ou de parties qui s’en détachent;
+• les dommages causés par des travaux d’extinction et de déblaiement;
+• disparition consécutive à ces événements:
+• les dommages de roussissement et les dommages aux choses assurées exposées involontairement à la chaleur.
+107.2 Restrictions de l’étendue de l’assurance
+Sont exclus de l’assurance les dommages causés à des machines, appareils et conduites sous tension par l’effet propre de l’électricité.
+113.2.3 Limitation des prestations pour les dommages de roussissement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>b) Prestation d’assurance «ALL RISK»
+Il n’existe pas de limitations particulières des prestations pour les dommages de roussissement et les dommages causés à des choses assurées qui ont été exposées involontairement à la chaleur.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,13 +637,34 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -419,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -441,6 +708,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,8 +1019,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -934,12 +1204,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -951,18 +1221,18 @@
         <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -971,21 +1241,21 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -997,7 +1267,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -1008,30 +1278,30 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
+      <c r="B13" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
@@ -1043,18 +1313,18 @@
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
@@ -1063,10 +1333,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
@@ -1076,8 +1346,8 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
+      <c r="B15" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
@@ -1089,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>11</v>
@@ -1100,7 +1370,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
@@ -1109,21 +1379,21 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
@@ -1135,7 +1405,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>11</v>
@@ -1146,7 +1416,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
@@ -1155,10 +1425,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>11</v>
@@ -1169,28 +1439,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="388" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
+      <c r="B20" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -1200,28 +1470,28 @@
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="388" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="356" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>11</v>

</xml_diff>